<commit_message>
add new test. upd checklist
</commit_message>
<xml_diff>
--- a/src/checklistStory4.xlsx
+++ b/src/checklistStory4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artyom_yuryshev/GIT/LEARN/ATM/atm-js-intermediate/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB9C7A8-F5F1-164C-8A7A-D07FF4653823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771B42A0-64BC-B245-BEF7-C4C8F85CEB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="24500" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{1C13D736-5A7C-214A-8A9D-7CE740893E32}"/>
+    <workbookView xWindow="4540" yWindow="24500" windowWidth="28800" windowHeight="16240" activeTab="2" xr2:uid="{1C13D736-5A7C-214A-8A9D-7CE740893E32}"/>
   </bookViews>
   <sheets>
     <sheet name="Сторя" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
   <si>
     <t>Summary</t>
   </si>
@@ -126,51 +126,12 @@
     </r>
   </si>
   <si>
-    <t>1) проверить, что юзер может открыть калькулятор для Compute Engine</t>
-  </si>
-  <si>
-    <t>2) проверить, что Estimated cost отображатеся для юзера в шапке страницы (дефолтный конфиг без изменений)</t>
-  </si>
-  <si>
-    <t>3) проверить, что Estimated cost отображатеся для юзера в Cost details  (дефолтный конфиг без изменений)</t>
-  </si>
-  <si>
-    <t>5) проверить, что юзер может изменять number of instances</t>
-  </si>
-  <si>
-    <t>6) проверить, что юзер может изменять disk size</t>
-  </si>
-  <si>
-    <t>7) проверить, что юзер может изменять OS</t>
-  </si>
-  <si>
-    <t>8) проверить, что калькуляцию стоимости (определённое значение при machine type of "n1-standard-1", number of instances as "2", disk size of "100GB", operating system as "Ubuntu 18.04")</t>
-  </si>
-  <si>
-    <t>9) проверить, что стоимость изменяется при изменении конфигурации ( с (machine type of "n1-standard-1", number of instances as "2", disk size of "100GB", operating system as "Ubuntu 18.04") на (machine type of "n1-standard-2"))</t>
-  </si>
-  <si>
     <t>позитив</t>
   </si>
   <si>
     <t>негатив</t>
   </si>
   <si>
-    <t>1) проверить, что юзер может открыть калькулятор для Cloud Storage</t>
-  </si>
-  <si>
-    <t>4) проверить, что стоимость изменяется при изменении конфигурации</t>
-  </si>
-  <si>
-    <t>1) проверить, что юзер может открыть калькулятор для BigQuery</t>
-  </si>
-  <si>
-    <t>1) проверить, что юзер может открыть калькулятор для Kubernetes Engine</t>
-  </si>
-  <si>
-    <t>4) проверить, что юзер может изменять machine type</t>
-  </si>
-  <si>
     <t>по 4 сторе я предагаю расширить чеклист, например:</t>
   </si>
   <si>
@@ -195,50 +156,92 @@
     <t>В целом т.к. тут много сочетаний разных дропдаунов и опций, то можно сгенерить что-то в копценпции попарного тестирования, например</t>
   </si>
   <si>
-    <t>11) Добавить в калькулятор Все Service Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12) Проверить, что можно удалять Айтемы из калькулятора </t>
-  </si>
-  <si>
-    <t xml:space="preserve">13) Проверить, что можно удалить Группу из калькулятора </t>
-  </si>
-  <si>
     <t>1) проверить, что Можно в калькулятор добавить одновременно Айтемы из Compute Engine, Cloud Storage, BigQuery и Kubernetes Engine</t>
   </si>
   <si>
-    <t>14) проверить, что валидацию number of instances  (Value needs to be greater than 0 and less than or equal to 50,000) (0 , 1, 49 999, 50 000, 50 001)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15) проверить, что юзер не может ввести невалидные данные (отрицательное значение/буквы/спецсивмолы) в number of instances </t>
-  </si>
-  <si>
-    <t>16) проверить валидацию Boot disk size (0 and less than or equal to 65,536 GiB) (ввод: 0, 1, 65 535, 65 536, 65 536)</t>
-  </si>
-  <si>
-    <t>17) проверить, что юзер не может ввести невалидные данные (отрицательное значение/буквы/спецсивмолы) в Boot disk size</t>
-  </si>
-  <si>
-    <t>10) Проверить содержимое Service type дроп-дауна</t>
-  </si>
-  <si>
-    <t>5) Проверить содержимое Service type дроп-дауна</t>
-  </si>
-  <si>
-    <t>6) Добавить в калькулятор Все Service Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7) Проверить, что можно удалять Айтемы из калькулятора </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8) Проверить, что можно удалить Группу из калькулятора </t>
+    <t>Реализовано в cloud-calculator.spec.ts</t>
+  </si>
+  <si>
+    <t>Комент</t>
+  </si>
+  <si>
+    <t>Реализовано в computeEngine.spec.ts</t>
+  </si>
+  <si>
+    <t>Проверить, что юзер может открыть калькулятор для Compute Engine</t>
+  </si>
+  <si>
+    <t>Проверить, что Estimated cost отображатеся для юзера в шапке страницы (дефолтный конфиг без изменений)</t>
+  </si>
+  <si>
+    <t>Проверить содержимое Machine Type DDL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Проверить, что Estimated cost отображатеся для юзера в Cost details  (дефолтный конфиг без изменений)</t>
+  </si>
+  <si>
+    <t>Проверить, что юзер может изменять machine type</t>
+  </si>
+  <si>
+    <t>Проверить, что юзер может изменять number of instances</t>
+  </si>
+  <si>
+    <t>Проверить, что юзер может изменять disk size</t>
+  </si>
+  <si>
+    <t>Проверить, что юзер может изменять OS</t>
+  </si>
+  <si>
+    <t>Проверить, что калькуляцию стоимости (определённое значение при machine type of "n1-standard-1", number of instances as "2", disk size of "100GB", operating system as "Ubuntu 18.04")</t>
+  </si>
+  <si>
+    <t>Проверить, что стоимость изменяется при изменении конфигурации ( с (machine type of "n1-standard-1", number of instances as "2", disk size of "100GB", operating system as "Ubuntu 18.04") на (machine type of "n1-standard-2"))</t>
+  </si>
+  <si>
+    <t>Проверить содержимое Service type дроп-дауна</t>
+  </si>
+  <si>
+    <t>Добавить в калькулятор Все Service Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Проверить, что можно удалять Айтемы из калькулятора </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Проверить, что можно удалить Группу из калькулятора </t>
+  </si>
+  <si>
+    <t>Проверить, что валидацию number of instances  (Value needs to be greater than 0 and less than or equal to 50,000) (0 , 1, 49 999, 50 000, 50 001)</t>
+  </si>
+  <si>
+    <t>Проверить валидацию Boot disk size (0 and less than or equal to 65,536 GiB) (ввод: 0, 1, 65 535, 65 536, 65 536)</t>
+  </si>
+  <si>
+    <t>Проверить, что юзер не может ввести невалидные данные (отрицательное значение/буквы/спецсивмолы) в Boot disk size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Проверить, что юзер не может ввести невалидные данные (отрицательное значение/буквы/спецсивмолы) в number of instances </t>
+  </si>
+  <si>
+    <t>Проверить, что юзер может открыть калькулятор для Cloud Storage</t>
+  </si>
+  <si>
+    <t>Проверить, что Estimated cost отображатеся для юзера в Cost details  (дефолтный конфиг без изменений)</t>
+  </si>
+  <si>
+    <t>Проверить, что стоимость изменяется при изменении конфигурации</t>
+  </si>
+  <si>
+    <t>Проверить, что юзер может открыть калькулятор для BigQuery</t>
+  </si>
+  <si>
+    <t>Проверить, что юзер может открыть калькулятор для Kubernetes Engine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -321,6 +324,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -343,7 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -361,6 +376,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -857,7 +883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E71F47-B330-F449-BEF4-F437E316A337}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -868,12 +894,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="24" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="46" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -883,110 +909,192 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4097EE4F-83B0-E642-B51E-DBBE96A9BBF5}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="186.33203125" customWidth="1"/>
+    <col min="2" max="2" width="156.83203125" customWidth="1"/>
+    <col min="3" max="3" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="C1" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="46" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="46" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="46" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="46" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="46" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="46" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="46" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" ht="22" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+    </row>
+    <row r="17" spans="1:2" ht="25" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="46" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="46" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="18" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>15</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A19" s="11">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="8"/>
-    </row>
-    <row r="16" spans="1:2" ht="25" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A20" s="11">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -997,60 +1105,85 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EF9743-4CCD-7348-9FD8-92A5CA6AC056}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A9"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="151.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="10"/>
+    <col min="2" max="2" width="151.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="3" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="5" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>53</v>
+    <row r="6" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1060,60 +1193,85 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9948C40B-514F-A240-B90D-2A591BA4EFF2}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A9"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="162.5" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="10"/>
+    <col min="2" max="2" width="162.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="5" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>53</v>
+    <row r="6" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1123,60 +1281,86 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E2422F-41E6-6A47-BDA6-8624E3788982}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="173.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="10"/>
+    <col min="2" max="2" width="173.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="13"/>
+      <c r="B1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="5" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="23" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>53</v>
+    <row r="6" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1196,42 +1380,42 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more tests, upd checklistStory4
</commit_message>
<xml_diff>
--- a/src/checklistStory4.xlsx
+++ b/src/checklistStory4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artyom_yuryshev/GIT/LEARN/ATM/atm-js-intermediate/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771B42A0-64BC-B245-BEF7-C4C8F85CEB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A93D87-A8D3-1141-82D4-7CA16EF16302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="24500" windowWidth="28800" windowHeight="16240" activeTab="2" xr2:uid="{1C13D736-5A7C-214A-8A9D-7CE740893E32}"/>
+    <workbookView xWindow="42900" yWindow="500" windowWidth="33900" windowHeight="22240" activeTab="2" xr2:uid="{1C13D736-5A7C-214A-8A9D-7CE740893E32}"/>
   </bookViews>
   <sheets>
     <sheet name="Сторя" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
   <si>
     <t>Summary</t>
   </si>
@@ -912,7 +912,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -984,28 +984,37 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="46" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+      <c r="C7" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="46" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+      <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="46" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>39</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="46" x14ac:dyDescent="0.3">
@@ -1015,6 +1024,9 @@
       <c r="B10" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="46" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
@@ -1023,13 +1035,16 @@
       <c r="B11" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="C11" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="23" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="23" x14ac:dyDescent="0.3">
@@ -1037,7 +1052,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="23" x14ac:dyDescent="0.3">
@@ -1045,33 +1060,32 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="23" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" ht="25" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:3" ht="22" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-    </row>
-    <row r="17" spans="1:2" ht="25" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="23" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>15</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>46</v>
+      <c r="B18" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="23" x14ac:dyDescent="0.3">
@@ -1079,7 +1093,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="23" x14ac:dyDescent="0.3">
@@ -1087,16 +1101,11 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
-        <v>18</v>
-      </c>
-      <c r="B21" s="5" t="s">
         <v>48</v>
       </c>
+    </row>
+    <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish positive test for computeEngine
</commit_message>
<xml_diff>
--- a/src/checklistStory4.xlsx
+++ b/src/checklistStory4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artyom_yuryshev/GIT/LEARN/ATM/atm-js-intermediate/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A93D87-A8D3-1141-82D4-7CA16EF16302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCC5C03-3478-6545-A55B-EBFF7A940F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42900" yWindow="500" windowWidth="33900" windowHeight="22240" activeTab="2" xr2:uid="{1C13D736-5A7C-214A-8A9D-7CE740893E32}"/>
+    <workbookView xWindow="-60" yWindow="-23500" windowWidth="33900" windowHeight="22220" activeTab="2" xr2:uid="{1C13D736-5A7C-214A-8A9D-7CE740893E32}"/>
   </bookViews>
   <sheets>
     <sheet name="Сторя" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>Summary</t>
   </si>
@@ -912,7 +912,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,28 +1039,37 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="46" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+      <c r="C12" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="46" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+      <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="46" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>45</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
finish tests for computeEngine
</commit_message>
<xml_diff>
--- a/src/checklistStory4.xlsx
+++ b/src/checklistStory4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artyom_yuryshev/GIT/LEARN/ATM/atm-js-intermediate/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCC5C03-3478-6545-A55B-EBFF7A940F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5242A556-711F-BE42-8967-266E8CFCA25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-23500" windowWidth="33900" windowHeight="22220" activeTab="2" xr2:uid="{1C13D736-5A7C-214A-8A9D-7CE740893E32}"/>
+    <workbookView xWindow="2120" yWindow="500" windowWidth="33900" windowHeight="22240" activeTab="2" xr2:uid="{1C13D736-5A7C-214A-8A9D-7CE740893E32}"/>
   </bookViews>
   <sheets>
     <sheet name="Сторя" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
   <si>
     <t>Summary</t>
   </si>
@@ -912,7 +912,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1081,39 +1081,51 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="46" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>14</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="C17" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="46" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="C18" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="46" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="23" x14ac:dyDescent="0.3">
+      <c r="C19" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="46" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="C20" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="22" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update checklistStory4 add new tests
</commit_message>
<xml_diff>
--- a/src/checklistStory4.xlsx
+++ b/src/checklistStory4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artyom_yuryshev/GIT/LEARN/ATM/atm-js-intermediate/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89190ECF-AEAD-5345-8AD9-3D05D95E7B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C66299-1576-D04B-AEEE-9611C8A7F67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22240" activeTab="2" xr2:uid="{1C13D736-5A7C-214A-8A9D-7CE740893E32}"/>
+    <workbookView xWindow="4500" yWindow="500" windowWidth="33900" windowHeight="22120" activeTab="2" xr2:uid="{1C13D736-5A7C-214A-8A9D-7CE740893E32}"/>
   </bookViews>
   <sheets>
     <sheet name="Сторя" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
   <si>
     <t>Summary</t>
   </si>
@@ -153,18 +153,6 @@
     <t>В целом т.к. тут много сочетаний разных дропдаунов и опций, то можно сгенерить что-то в копценпции попарного тестирования, например</t>
   </si>
   <si>
-    <t>1) проверить, что Можно в калькулятор добавить одновременно Айтемы из Compute Engine, Cloud Storage, BigQuery и Kubernetes Engine</t>
-  </si>
-  <si>
-    <t>Реализовано в cloud-calculator.spec.ts</t>
-  </si>
-  <si>
-    <t>Комент</t>
-  </si>
-  <si>
-    <t>Реализовано в computeEngine.spec.ts</t>
-  </si>
-  <si>
     <t>Проверить, что юзер может открыть калькулятор для Compute Engine</t>
   </si>
   <si>
@@ -216,13 +204,37 @@
     <t xml:space="preserve">Проверить, что юзер не может ввести невалидные данные (отрицательное значение/буквы/спецсивмолы) в number of instances </t>
   </si>
   <si>
-    <t>Undo Deleting</t>
-  </si>
-  <si>
     <t>Проверить содержимое Info Buttons</t>
   </si>
   <si>
     <t>Проверить возможность смены валюты</t>
+  </si>
+  <si>
+    <t>Проверить, что появляется нотификация об удалении</t>
+  </si>
+  <si>
+    <t>Проверить что можно отменить удаление (Undo Deleting)</t>
+  </si>
+  <si>
+    <t>Проверить, что появляется попап с подтверждением удаления группы айтемов</t>
+  </si>
+  <si>
+    <t>Проверить, что можно отменить процесс удаления группы айтемов</t>
+  </si>
+  <si>
+    <t>комент</t>
+  </si>
+  <si>
+    <t>Проверить, что Можно в калькулятор добавить одновременно Айтемы из Compute Engine, Cloud Storage, BigQuery и Kubernetes Engine</t>
+  </si>
+  <si>
+    <t>Реализовано в src/tests/smoke/multiple-types.spec.ts</t>
+  </si>
+  <si>
+    <t>Реализовано в src/tests/smoke/cloud-calculator.spec.ts</t>
+  </si>
+  <si>
+    <t>Реализовано в src/tests/regress/computeEngine.spec.ts</t>
   </si>
 </sst>
 </file>
@@ -300,15 +312,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFD93025"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -333,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -349,12 +362,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -849,26 +870,160 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E71F47-B330-F449-BEF4-F437E316A337}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="106.1640625" customWidth="1"/>
+    <col min="2" max="2" width="106.1640625" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="46" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="C1" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="69" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -877,16 +1032,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4097EE4F-83B0-E642-B51E-DBBE96A9BBF5}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="156.83203125" customWidth="1"/>
-    <col min="3" max="3" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.2">
@@ -894,231 +1049,270 @@
         <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C7" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="C9" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="C10" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="C11" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="C12" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="C13" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="C14" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A18" s="9">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A19" s="9">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="25" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A22" s="9">
+        <v>20</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A23" s="9">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A24" s="9">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="C24" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A25" s="9">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="23" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:3" ht="23" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:3" ht="23" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
-        <v>16</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:3" ht="25" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
-        <v>17</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
-        <v>18</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
-        <v>19</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="46" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
-        <v>20</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="22" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
+      <c r="C25" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="22" x14ac:dyDescent="0.2">
+      <c r="A26" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>